<commit_message>
Update BOM, start treebuilders
</commit_message>
<xml_diff>
--- a/PCB/PCBv1.0/bq25505 calc.xlsx
+++ b/PCB/PCBv1.0/bq25505 calc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Veridian-Heliograph\PCB\PCBv1.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8FA69BE-D4E3-4E03-9AC7-2E53A9CF7A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E355ED0-818E-45BC-9886-6B9F6A72EB0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2985" yWindow="2985" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bq25505(70" sheetId="1" r:id="rId1"/>
@@ -2234,7 +2234,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Y15" sqref="Y15"/>
+      <selection pane="topRight" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3003,7 +3003,7 @@
         <v>15</v>
       </c>
       <c r="C19" s="13">
-        <v>4.32</v>
+        <v>4.3</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>58</v>
@@ -3177,14 +3177,14 @@
       </c>
       <c r="C23" s="64">
         <f>$C$1*(1+C20/C19)*3/2</f>
-        <v>5.4534027777777769</v>
+        <v>5.4703255813953486</v>
       </c>
       <c r="D23" s="86" t="s">
         <v>1</v>
       </c>
       <c r="E23" s="65">
         <f>(C23-C9)/C23*100</f>
-        <v>-0.85446140916096247</v>
+        <v>-0.54246165357276832</v>
       </c>
       <c r="F23" s="84" t="s">
         <v>2</v>
@@ -4274,21 +4274,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Tag xmlns="e6b6f262-197a-43d7-8cc8-2398f9beca90" xsi:nil="true"/>
     <Thumbnail xmlns="e6b6f262-197a-43d7-8cc8-2398f9beca90" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4529,19 +4529,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{455C7BEF-6E75-4721-857D-8DB037DB4B67}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{276C0D19-B21D-4E63-AC38-166F7A170215}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="e6b6f262-197a-43d7-8cc8-2398f9beca90"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{455C7BEF-6E75-4721-857D-8DB037DB4B67}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>